<commit_message>
Grupo6: Caso de Teste
</commit_message>
<xml_diff>
--- a/grupo6/Casos de Testes - Grupo 6.xlsx
+++ b/grupo6/Casos de Testes - Grupo 6.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Entrada (Salário; Qtde de dependentes)</t>
   </si>
@@ -49,7 +49,28 @@
     <t xml:space="preserve">Sal:3000;QtdDep:3</t>
   </si>
   <si>
-    <t xml:space="preserve">INSS:330;FGTS:240;ALIQ:2106;IR:15,19;SAL.LIQ:2414,81</t>
+    <t xml:space="preserve">INSS:330;FGTS:240;ALIQ:2106;IR:15,19;SAL.LIQ:2414,81;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sal:800;QtdDep:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSS:64;FGTS:64;ALIQ:548,20;IR:INSENTO;SAL.LIQ:672;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sal:1750;QtdDep:6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSS:157,50;FGTS:140;ALIQ:465,70;IR:INSENTO;SAL.LIQ:1452,50;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sal:4500;QtdDep:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSS:495;FGTS:360;ALIQ:3629,40;IR:189,61:SAL.LIQ:3455,39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSS</t>
   </si>
 </sst>
 </file>
@@ -158,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -211,6 +232,35 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>